<commit_message>
Updated project files and added new features
</commit_message>
<xml_diff>
--- a/failed_log.xlsx
+++ b/failed_log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,177 +448,33 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>201024374628</t>
+          <t>201032822563</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//div[@contenteditable="true"][@data-tab="3"]"}
-  (Session info: chrome=141.0.7390.108); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#nosuchelementexception
+          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//div[@contenteditable="true"][@data-tab="10"]"}
+  (Session info: chrome=141.0.7390.108); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
 Stacktrace:
-	GetHandleVerifier [0x0x7ff696aee9e5+80021]
-	GetHandleVerifier [0x0x7ff696aeea40+80112]
-	(No symbol) [0x0x7ff69687060f]
-	(No symbol) [0x0x7ff6968c8854]
-	(No symbol) [0x0x7ff6968c8b1c]
-	(No symbol) [0x0x7ff69691c927]
-	(No symbol) [0x0x7ff6968f126f]
-	(No symbol) [0x0x7ff69691968a]
-	(No symbol) [0x0x7ff6968f1003]
-	(No symbol) [0x0x7ff6968b95d1]
-	(No symbol) [0x0x7ff6968ba3f3]
-	GetHandleVerifier [0x0x7ff696dadd8d+2960445]
-	GetHandleVerifier [0x0x7ff696da804a+2936570]
-	GetHandleVerifier [0x0x7ff696dc8a87+3070263]
-	GetHandleVerifier [0x0x7ff696b084ce+185214]
-	GetHandleVerifier [0x0x7ff696b0ff1f+216527]
-	GetHandleVerifier [0x0x7ff696af7c24+117460]
-	GetHandleVerifier [0x0x7ff696af7ddf+117903]
-	GetHandleVerifier [0x0x7ff696addcb8+11112]
-	BaseThreadInitThunk [0x0x7ff9476be8d7+23]
-	RtlUserThreadStart [0x0x7ff94821c34c+44]
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>201550301267</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//div[@contenteditable="true"][@data-tab="3"]"}
-  (Session info: chrome=141.0.7390.108); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#nosuchelementexception
-Stacktrace:
-	GetHandleVerifier [0x0x7ff696aee9e5+80021]
-	GetHandleVerifier [0x0x7ff696aeea40+80112]
-	(No symbol) [0x0x7ff69687060f]
-	(No symbol) [0x0x7ff6968c8854]
-	(No symbol) [0x0x7ff6968c8b1c]
-	(No symbol) [0x0x7ff69691c927]
-	(No symbol) [0x0x7ff6968f126f]
-	(No symbol) [0x0x7ff69691968a]
-	(No symbol) [0x0x7ff6968f1003]
-	(No symbol) [0x0x7ff6968b95d1]
-	(No symbol) [0x0x7ff6968ba3f3]
-	GetHandleVerifier [0x0x7ff696dadd8d+2960445]
-	GetHandleVerifier [0x0x7ff696da804a+2936570]
-	GetHandleVerifier [0x0x7ff696dc8a87+3070263]
-	GetHandleVerifier [0x0x7ff696b084ce+185214]
-	GetHandleVerifier [0x0x7ff696b0ff1f+216527]
-	GetHandleVerifier [0x0x7ff696af7c24+117460]
-	GetHandleVerifier [0x0x7ff696af7ddf+117903]
-	GetHandleVerifier [0x0x7ff696addcb8+11112]
-	BaseThreadInitThunk [0x0x7ff9476be8d7+23]
-	RtlUserThreadStart [0x0x7ff94821c34c+44]
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>201032822563</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//div[@contenteditable="true"][@data-tab="3"]"}
-  (Session info: chrome=141.0.7390.108); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#nosuchelementexception
-Stacktrace:
-	GetHandleVerifier [0x0x7ff696aee9e5+80021]
-	GetHandleVerifier [0x0x7ff696aeea40+80112]
-	(No symbol) [0x0x7ff69687060f]
-	(No symbol) [0x0x7ff6968c8854]
-	(No symbol) [0x0x7ff6968c8b1c]
-	(No symbol) [0x0x7ff69691c927]
-	(No symbol) [0x0x7ff6968f126f]
-	(No symbol) [0x0x7ff69691968a]
-	(No symbol) [0x0x7ff6968f1003]
-	(No symbol) [0x0x7ff6968b95d1]
-	(No symbol) [0x0x7ff6968ba3f3]
-	GetHandleVerifier [0x0x7ff696dadd8d+2960445]
-	GetHandleVerifier [0x0x7ff696da804a+2936570]
-	GetHandleVerifier [0x0x7ff696dc8a87+3070263]
-	GetHandleVerifier [0x0x7ff696b084ce+185214]
-	GetHandleVerifier [0x0x7ff696b0ff1f+216527]
-	GetHandleVerifier [0x0x7ff696af7c24+117460]
-	GetHandleVerifier [0x0x7ff696af7ddf+117903]
-	GetHandleVerifier [0x0x7ff696addcb8+11112]
-	BaseThreadInitThunk [0x0x7ff9476be8d7+23]
-	RtlUserThreadStart [0x0x7ff94821c34c+44]
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>201550301267</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//div[@contenteditable="true"][@data-tab="3"]"}
-  (Session info: chrome=141.0.7390.108); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#nosuchelementexception
-Stacktrace:
-	GetHandleVerifier [0x0x7ff696aee9e5+80021]
-	GetHandleVerifier [0x0x7ff696aeea40+80112]
-	(No symbol) [0x0x7ff69687060f]
-	(No symbol) [0x0x7ff6968c8854]
-	(No symbol) [0x0x7ff6968c8b1c]
-	(No symbol) [0x0x7ff69691c927]
-	(No symbol) [0x0x7ff6968f126f]
-	(No symbol) [0x0x7ff69691968a]
-	(No symbol) [0x0x7ff6968f1003]
-	(No symbol) [0x0x7ff6968b95d1]
-	(No symbol) [0x0x7ff6968ba3f3]
-	GetHandleVerifier [0x0x7ff696dadd8d+2960445]
-	GetHandleVerifier [0x0x7ff696da804a+2936570]
-	GetHandleVerifier [0x0x7ff696dc8a87+3070263]
-	GetHandleVerifier [0x0x7ff696b084ce+185214]
-	GetHandleVerifier [0x0x7ff696b0ff1f+216527]
-	GetHandleVerifier [0x0x7ff696af7c24+117460]
-	GetHandleVerifier [0x0x7ff696af7ddf+117903]
-	GetHandleVerifier [0x0x7ff696addcb8+11112]
-	BaseThreadInitThunk [0x0x7ff9476be8d7+23]
-	RtlUserThreadStart [0x0x7ff94821c34c+44]
-</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>201150665030</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//div[@contenteditable="true"][@data-tab="3"]"}
-  (Session info: chrome=141.0.7390.108); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#nosuchelementexception
-Stacktrace:
-	GetHandleVerifier [0x0x7ff696aee9e5+80021]
-	GetHandleVerifier [0x0x7ff696aeea40+80112]
-	(No symbol) [0x0x7ff69687060f]
-	(No symbol) [0x0x7ff6968c8854]
-	(No symbol) [0x0x7ff6968c8b1c]
-	(No symbol) [0x0x7ff69691c927]
-	(No symbol) [0x0x7ff6968f126f]
-	(No symbol) [0x0x7ff69691968a]
-	(No symbol) [0x0x7ff6968f1003]
-	(No symbol) [0x0x7ff6968b95d1]
-	(No symbol) [0x0x7ff6968ba3f3]
-	GetHandleVerifier [0x0x7ff696dadd8d+2960445]
-	GetHandleVerifier [0x0x7ff696da804a+2936570]
-	GetHandleVerifier [0x0x7ff696dc8a87+3070263]
-	GetHandleVerifier [0x0x7ff696b084ce+185214]
-	GetHandleVerifier [0x0x7ff696b0ff1f+216527]
-	GetHandleVerifier [0x0x7ff696af7c24+117460]
-	GetHandleVerifier [0x0x7ff696af7ddf+117903]
-	GetHandleVerifier [0x0x7ff696addcb8+11112]
+	GetHandleVerifier [0x0x7ff607dce9e5+80021]
+	GetHandleVerifier [0x0x7ff607dcea40+80112]
+	(No symbol) [0x0x7ff607b5060f]
+	(No symbol) [0x0x7ff607ba8854]
+	(No symbol) [0x0x7ff607ba8b1c]
+	(No symbol) [0x0x7ff607bfc927]
+	(No symbol) [0x0x7ff607bd126f]
+	(No symbol) [0x0x7ff607bf968a]
+	(No symbol) [0x0x7ff607bd1003]
+	(No symbol) [0x0x7ff607b995d1]
+	(No symbol) [0x0x7ff607b9a3f3]
+	GetHandleVerifier [0x0x7ff60808dd8d+2960445]
+	GetHandleVerifier [0x0x7ff60808804a+2936570]
+	GetHandleVerifier [0x0x7ff6080a8a87+3070263]
+	GetHandleVerifier [0x0x7ff607de84ce+185214]
+	GetHandleVerifier [0x0x7ff607deff1f+216527]
+	GetHandleVerifier [0x0x7ff607dd7c24+117460]
+	GetHandleVerifier [0x0x7ff607dd7ddf+117903]
+	GetHandleVerifier [0x0x7ff607dbdcb8+11112]
 	BaseThreadInitThunk [0x0x7ff9476be8d7+23]
 	RtlUserThreadStart [0x0x7ff94821c34c+44]
 </t>

</xml_diff>

<commit_message>
Updated project files and added new features v2
</commit_message>
<xml_diff>
--- a/failed_log.xlsx
+++ b/failed_log.xlsx
@@ -453,31 +453,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Message: no such element: Unable to locate element: {"method":"xpath","selector":"//div[@contenteditable="true"][@data-tab="10"]"}
-  (Session info: chrome=141.0.7390.108); For documentation on this error, please visit: https://www.selenium.dev/documentation/webdriver/troubleshooting/errors#no-such-element-exception
-Stacktrace:
-	GetHandleVerifier [0x0x7ff607dce9e5+80021]
-	GetHandleVerifier [0x0x7ff607dcea40+80112]
-	(No symbol) [0x0x7ff607b5060f]
-	(No symbol) [0x0x7ff607ba8854]
-	(No symbol) [0x0x7ff607ba8b1c]
-	(No symbol) [0x0x7ff607bfc927]
-	(No symbol) [0x0x7ff607bd126f]
-	(No symbol) [0x0x7ff607bf968a]
-	(No symbol) [0x0x7ff607bd1003]
-	(No symbol) [0x0x7ff607b995d1]
-	(No symbol) [0x0x7ff607b9a3f3]
-	GetHandleVerifier [0x0x7ff60808dd8d+2960445]
-	GetHandleVerifier [0x0x7ff60808804a+2936570]
-	GetHandleVerifier [0x0x7ff6080a8a87+3070263]
-	GetHandleVerifier [0x0x7ff607de84ce+185214]
-	GetHandleVerifier [0x0x7ff607deff1f+216527]
-	GetHandleVerifier [0x0x7ff607dd7c24+117460]
-	GetHandleVerifier [0x0x7ff607dd7ddf+117903]
-	GetHandleVerifier [0x0x7ff607dbdcb8+11112]
-	BaseThreadInitThunk [0x0x7ff9476be8d7+23]
-	RtlUserThreadStart [0x0x7ff94821c34c+44]
-</t>
+          <t>Invalid WhatsApp number</t>
         </is>
       </c>
     </row>

</xml_diff>